<commit_message>
Update THONG BAO BIEN DONG GOI XA_BPKT.xls
</commit_message>
<xml_diff>
--- a/SODO/Khe Sanh/FixedRowCopy.xlsx
+++ b/SODO/Khe Sanh/FixedRowCopy.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Số tờ</t>
   </si>
@@ -116,31 +116,34 @@
     <t>Cấp đổi</t>
   </si>
   <si>
-    <t>Khối 3A, thị trấn Khe Sanh, huyện Hướng Hóa, tỉnh Quảng Trị</t>
+    <t>950,6</t>
   </si>
   <si>
-    <t>ODT</t>
+    <t>Khối 1, thị trấn Khe Sanh, huyện Hướng Hóa, tỉnh Quảng Trị</t>
   </si>
   <si>
-    <t>CLN</t>
+    <t>Bà Dương Thị Loan và ông Ngô Ngọc Quý</t>
   </si>
   <si>
-    <t>Hộ bà Đinh Thị Thơi</t>
+    <t>26/03/2013</t>
   </si>
   <si>
-    <t>27/12/2021</t>
+    <t>BL 832370</t>
   </si>
   <si>
-    <t>U 577726</t>
+    <t>giảm 3,3</t>
   </si>
   <si>
-    <t>giảm 35,4</t>
+    <t>1279/24</t>
   </si>
   <si>
-    <t>146,2</t>
+    <t>0973295409</t>
   </si>
   <si>
-    <t>0917565111</t>
+    <t>Đô Thị</t>
+  </si>
+  <si>
+    <t>1409/23</t>
   </si>
 </sst>
 </file>
@@ -192,7 +195,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -215,11 +218,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -239,17 +257,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7956,6 +7977,71 @@
     <xdr:sp macro="[1]!Form" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="120" name="Rounded Rectangle 119"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="38100" y="57150"/>
+          <a:ext cx="581025" cy="371475"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>FORM</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>428625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="[1]!Form" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="121" name="Rounded Rectangle 120"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -8307,7 +8393,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:29" s="6" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" s="6" customFormat="1" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8393,72 +8479,74 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" ht="111" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="B2" s="7">
-        <v>50</v>
+        <v>7</v>
       </c>
-      <c r="C2" s="8">
-        <v>1215.5999999999999</v>
-      </c>
-      <c r="D2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="7">
-        <v>1</v>
-      </c>
-      <c r="F2" s="7" t="s">
+      <c r="D2" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="9">
-        <v>300</v>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="8">
+        <v>250</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="7"/>
+      <c r="I2" s="8">
+        <v>9256</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="9">
-        <v>915.59999999999991</v>
+      <c r="K2" s="7" t="s">
+        <v>30</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="L2" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="L2" s="7" t="s">
+      <c r="M2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="N2" s="7"/>
+      <c r="O2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="N2" s="7">
-        <v>1251</v>
+      <c r="P2" s="7">
+        <v>141</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="Q2" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="R2" s="11" t="s">
         <v>36</v>
-      </c>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="10" t="s">
-        <v>37</v>
       </c>
       <c r="S2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="T2" s="7"/>
+      <c r="T2" s="7" t="s">
+        <v>37</v>
+      </c>
       <c r="U2" s="7"/>
       <c r="V2" s="7"/>
-      <c r="W2" s="7"/>
-      <c r="X2" s="7"/>
+      <c r="W2" s="7">
+        <v>50</v>
+      </c>
+      <c r="X2" s="7">
+        <v>7</v>
+      </c>
       <c r="Y2" s="7"/>
       <c r="Z2" s="7"/>
       <c r="AA2" s="7"/>
       <c r="AB2" s="7"/>
-      <c r="AC2" s="7"/>
+      <c r="AC2" s="7" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>